<commit_message>
Split certificates into certificates (final products) and documents (word document for certificates)
</commit_message>
<xml_diff>
--- a/student-final/Registers/register.xlsx
+++ b/student-final/Registers/register.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nr. adeverinta</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Bursa</t>
+  </si>
+  <si>
+    <t>11/01/2024</t>
+  </si>
+  <si>
+    <t>spitalizare</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:N30"/>
@@ -527,6 +533,26 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="0">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Finished proof of concept
</commit_message>
<xml_diff>
--- a/student-final/Registers/register.xlsx
+++ b/student-final/Registers/register.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nr. adeverinta</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>spitalizare</t>
+  </si>
+  <si>
+    <t>marian vrea adeverinta</t>
+  </si>
+  <si>
+    <t>bursa</t>
   </si>
 </sst>
 </file>
@@ -437,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:N30"/>
@@ -553,6 +559,46 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="0">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Added removing document after sending email functionality
</commit_message>
<xml_diff>
--- a/student-final/Registers/register.xlsx
+++ b/student-final/Registers/register.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Nr. adeverinta</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>bursa</t>
+  </si>
+  <si>
+    <t>camin</t>
+  </si>
+  <si>
+    <t>Cristian</t>
+  </si>
+  <si>
+    <t>abonament de autobuz</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -443,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:N30"/>
@@ -599,6 +614,186 @@
         <v>18</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="0">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="0">
+        <v>2</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="0">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="0">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="0">
+        <v>2</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="0">
+        <v>2</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="0">
+        <v>2</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="0">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>